<commit_message>
English transcription, alphabet and intro to OpenCart
</commit_message>
<xml_diff>
--- a/content/english/content/dictionary/dictionary.xlsx
+++ b/content/english/content/dictionary/dictionary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>Word</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">attribute  </t>
   </si>
   <si>
-    <t xml:space="preserve">bolean     </t>
-  </si>
-  <si>
     <t xml:space="preserve">controller </t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t xml:space="preserve">view       </t>
   </si>
   <si>
-    <t xml:space="preserve">массив     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">атрибут    </t>
-  </si>
-  <si>
     <t xml:space="preserve">           </t>
   </si>
   <si>
@@ -112,12 +103,6 @@
     <t>база данных</t>
   </si>
   <si>
-    <t xml:space="preserve">тогда      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">выполнять  </t>
-  </si>
-  <si>
     <t xml:space="preserve">функция    </t>
   </si>
   <si>
@@ -170,6 +155,81 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>[ə'reɪ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">массив, набор    </t>
+  </si>
+  <si>
+    <t>['ætrɪbjuːt]</t>
+  </si>
+  <si>
+    <t>атрибут, свойство</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean     </t>
+  </si>
+  <si>
+    <t>[ˈbuːlɪən]</t>
+  </si>
+  <si>
+    <t>булев, логический</t>
+  </si>
+  <si>
+    <t>[kən'trəulə]</t>
+  </si>
+  <si>
+    <t>['deɪtəbeɪs]</t>
+  </si>
+  <si>
+    <t>['elɪfənt]</t>
+  </si>
+  <si>
+    <t>слон</t>
+  </si>
+  <si>
+    <t>[els]</t>
+  </si>
+  <si>
+    <t>иначе</t>
+  </si>
+  <si>
+    <t>['eksɪkjuːt]</t>
+  </si>
+  <si>
+    <t>выполнять, реализововать</t>
+  </si>
+  <si>
+    <t>выполнять, исполнять</t>
+  </si>
+  <si>
+    <t>['fʌŋkʃ(ə)n]</t>
+  </si>
+  <si>
+    <t>implement</t>
+  </si>
+  <si>
+    <t>['ɪmplɪmənt]</t>
+  </si>
+  <si>
+    <t>переменная</t>
+  </si>
+  <si>
+    <t>[puʃ]</t>
+  </si>
+  <si>
+    <t>проталкивать</t>
+  </si>
+  <si>
+    <t>извлекать</t>
+  </si>
+  <si>
+    <t>[pul]</t>
+  </si>
+  <si>
+    <t>[ɪf]</t>
   </si>
 </sst>
 </file>
@@ -198,7 +258,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,18 +274,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -266,14 +314,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,7 +625,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,31 +635,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -622,292 +670,335 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>